<commit_message>
Correlation: analiz dependent columns
</commit_message>
<xml_diff>
--- a/reports/correlation/Pearson_correlation_backgrounds.xlsx
+++ b/reports/correlation/Pearson_correlation_backgrounds.xlsx
@@ -4,18 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="23955" windowHeight="9780" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="135" windowWidth="23955" windowHeight="9780" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Коэффициент корреляции" sheetId="1" r:id="rId1"/>
     <sheet name="Уровень значимости" sheetId="2" r:id="rId2"/>
+    <sheet name="Корреляция более 75%" sheetId="3" r:id="rId3"/>
+    <sheet name="Корреляция более 80%" sheetId="4" r:id="rId4"/>
+    <sheet name="Корреляция более 85%" sheetId="5" r:id="rId5"/>
+    <sheet name="Корреляция более 90%" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1920" uniqueCount="820">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1956" uniqueCount="836">
   <si>
     <t>DER_mass_MMC</t>
   </si>
@@ -2475,6 +2479,54 @@
   </si>
   <si>
     <t>0.522052678842</t>
+  </si>
+  <si>
+    <t>3 DER_pt_h 9 DER_sum_pt (0.80465631268380367, 0.0)</t>
+  </si>
+  <si>
+    <t>3 DER_pt_h 21 PRI_met_sumet (0.76295643297226268, 0.0)</t>
+  </si>
+  <si>
+    <t>3 DER_pt_h 29 PRI_jet_all_pt (0.78030514800037387, 0.0)</t>
+  </si>
+  <si>
+    <t>9 DER_sum_pt 21 PRI_met_sumet (0.90136734493390336, 0.0)</t>
+  </si>
+  <si>
+    <t>9 DER_sum_pt 22 PRI_jet_num (0.77381750235404123, 0.0)</t>
+  </si>
+  <si>
+    <t>9 DER_sum_pt 29 PRI_jet_all_pt (0.96300530649741123, 0.0)</t>
+  </si>
+  <si>
+    <t>21 PRI_met_sumet 29 PRI_jet_all_pt (0.88153096941468034, 0.0)</t>
+  </si>
+  <si>
+    <t>22 PRI_jet_num 29 PRI_jet_all_pt (0.81379266838833642, 0.0)</t>
+  </si>
+  <si>
+    <t>9 DER_sum_pt 3 DER_pt_h (0.80465631268380367, 0.0)</t>
+  </si>
+  <si>
+    <t>21 PRI_met_sumet 3 DER_pt_h (0.76295643297226268, 0.0)</t>
+  </si>
+  <si>
+    <t>21 PRI_met_sumet 9 DER_sum_pt (0.90136734493390336, 0.0)</t>
+  </si>
+  <si>
+    <t>22 PRI_jet_num 9 DER_sum_pt (0.77381750235404123, 0.0)</t>
+  </si>
+  <si>
+    <t>29 PRI_jet_all_pt 3 DER_pt_h (0.78030514800037387, 0.0)</t>
+  </si>
+  <si>
+    <t>29 PRI_jet_all_pt 9 DER_sum_pt (0.96300530649741123, 0.0)</t>
+  </si>
+  <si>
+    <t>29 PRI_jet_all_pt 21 PRI_met_sumet (0.88153096941468034, 0.0)</t>
+  </si>
+  <si>
+    <t>29 PRI_jet_all_pt 22 PRI_jet_num (0.81379266838833642, 0.0)</t>
   </si>
 </sst>
 </file>
@@ -3337,8 +3389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE31"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection sqref="A1:AE31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6302,8 +6354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9260,4 +9312,305 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>820</v>
+      </c>
+      <c r="J1">
+        <v>3</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>21</v>
+      </c>
+      <c r="M1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>821</v>
+      </c>
+      <c r="J2">
+        <v>9</v>
+      </c>
+      <c r="K2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>822</v>
+      </c>
+      <c r="J3">
+        <v>29</v>
+      </c>
+      <c r="K3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" t="s">
+        <v>835</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>820</v>
+      </c>
+      <c r="J1">
+        <v>3</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>828</v>
+      </c>
+      <c r="J2">
+        <v>9</v>
+      </c>
+      <c r="K2">
+        <v>21</v>
+      </c>
+      <c r="L2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>823</v>
+      </c>
+      <c r="J3">
+        <v>22</v>
+      </c>
+      <c r="K3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>835</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>823</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>21</v>
+      </c>
+      <c r="L1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>834</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>823</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>21</v>
+      </c>
+      <c r="L1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>833</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>